<commit_message>
FAQs, Embroidery Base Price Calculation, Dynamic Embroidery Base Price Calculations
</commit_message>
<xml_diff>
--- a/costing.xlsx
+++ b/costing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tayaw\Desktop\Projects\mayhem-creations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A6A63A8D-4A41-4178-AB23-75706FD9A7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D82DB96-E2C7-454F-84E7-69B0A99286AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1073" yWindow="1073" windowWidth="16200" windowHeight="9307" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Material" sheetId="1" r:id="rId1"/>
@@ -452,7 +452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -586,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -621,7 +621,7 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>50000</v>
       </c>
     </row>
   </sheetData>
@@ -634,7 +634,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -671,7 +671,7 @@
       </c>
       <c r="B4">
         <f>ROUND((Input!B4 / 1000000) * Material!B4 * Material!E4, 2)</f>
-        <v>0</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
@@ -680,7 +680,7 @@
       </c>
       <c r="B5">
         <f>ROUND((Input!B4 / Material!D5) * (Material!B5 / 144) * Material!E5, 2)</f>
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
@@ -707,7 +707,7 @@
       </c>
       <c r="B8">
         <f>SUM(B2:B7)</f>
-        <v>0.43000000000000005</v>
+        <v>1.27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>